<commit_message>
adding to todo list abilities
</commit_message>
<xml_diff>
--- a/reviewerTodoList.xlsx
+++ b/reviewerTodoList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukel\Documents\phdThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA6D7AF-95E3-4229-89E6-7AA1D0D08B44}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FEAAE1-C84D-4178-B614-C031AA797C56}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6792" xr2:uid="{D14D4B82-700B-4764-8F82-CFD1564063A2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>ID</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>signpostign and summaries on conclusions and intros (revert to research questions)</t>
+  </si>
+  <si>
+    <t>PERCENT COMPLETE</t>
   </si>
 </sst>
 </file>
@@ -242,10 +245,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -561,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784CD99F-F0D7-4557-AEAE-23B01A0F6CDF}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -573,7 +579,7 @@
     <col min="3" max="3" width="98.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -587,7 +593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <f>0</f>
         <v>0</v>
@@ -601,8 +607,12 @@
       <c r="D2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2">
+        <f>IF(D2,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
@@ -616,10 +626,14 @@
       <c r="D3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E3">
+        <f t="shared" ref="E3:E55" si="0">IF(D3,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
-        <f t="shared" ref="A4:A55" si="0">A3+1</f>
+        <f t="shared" ref="A4:A55" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4">
@@ -631,10 +645,14 @@
       <c r="D4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B5">
@@ -646,10 +664,14 @@
       <c r="D5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B6">
@@ -661,10 +683,14 @@
       <c r="D6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B7">
@@ -676,10 +702,14 @@
       <c r="D7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B8">
@@ -691,10 +721,14 @@
       <c r="D8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B9">
@@ -706,10 +740,14 @@
       <c r="D9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B10">
@@ -721,10 +759,14 @@
       <c r="D10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B11">
@@ -736,10 +778,14 @@
       <c r="D11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B12">
@@ -751,10 +797,14 @@
       <c r="D12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B13">
@@ -766,10 +816,14 @@
       <c r="D13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B14">
@@ -781,10 +835,14 @@
       <c r="D14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B15">
@@ -796,10 +854,14 @@
       <c r="D15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B16">
@@ -811,10 +873,14 @@
       <c r="D16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B17">
@@ -826,10 +892,14 @@
       <c r="D17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B18">
@@ -841,10 +911,14 @@
       <c r="D18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B19">
@@ -856,10 +930,14 @@
       <c r="D19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B20">
@@ -871,10 +949,14 @@
       <c r="D20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B21">
@@ -886,10 +968,14 @@
       <c r="D21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B22">
@@ -901,10 +987,14 @@
       <c r="D22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B23">
@@ -916,10 +1006,14 @@
       <c r="D23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B24">
@@ -931,10 +1025,14 @@
       <c r="D24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B25">
@@ -946,10 +1044,14 @@
       <c r="D25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B26">
@@ -961,10 +1063,14 @@
       <c r="D26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B27">
@@ -976,10 +1082,14 @@
       <c r="D27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B28">
@@ -991,10 +1101,14 @@
       <c r="D28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B29">
@@ -1006,10 +1120,14 @@
       <c r="D29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B30">
@@ -1021,10 +1139,14 @@
       <c r="D30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B31">
@@ -1036,10 +1158,14 @@
       <c r="D31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B32">
@@ -1051,10 +1177,14 @@
       <c r="D32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B33">
@@ -1066,10 +1196,14 @@
       <c r="D33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B34">
@@ -1081,10 +1215,14 @@
       <c r="D34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B35">
@@ -1096,10 +1234,14 @@
       <c r="D35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B36">
@@ -1111,10 +1253,14 @@
       <c r="D36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B37">
@@ -1126,10 +1272,14 @@
       <c r="D37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B38">
@@ -1141,10 +1291,14 @@
       <c r="D38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B39">
@@ -1156,10 +1310,14 @@
       <c r="D39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B40">
@@ -1171,10 +1329,14 @@
       <c r="D40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B41">
@@ -1186,10 +1348,14 @@
       <c r="D41" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B42">
@@ -1201,10 +1367,14 @@
       <c r="D42" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B43">
@@ -1216,10 +1386,14 @@
       <c r="D43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B44">
@@ -1231,10 +1405,14 @@
       <c r="D44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B45">
@@ -1246,10 +1424,14 @@
       <c r="D45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B46">
@@ -1261,10 +1443,14 @@
       <c r="D46" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B47">
@@ -1276,10 +1462,14 @@
       <c r="D47" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B48">
@@ -1291,10 +1481,14 @@
       <c r="D48" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B49">
@@ -1306,10 +1500,14 @@
       <c r="D49" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B50">
@@ -1321,10 +1519,14 @@
       <c r="D50" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B51">
@@ -1336,10 +1538,14 @@
       <c r="D51" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B52">
@@ -1351,10 +1557,14 @@
       <c r="D52" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B53">
@@ -1366,10 +1576,14 @@
       <c r="D53" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B54" t="s">
@@ -1381,10 +1595,14 @@
       <c r="D54" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B55" t="s">
@@ -1394,6 +1612,19 @@
         <v>58</v>
       </c>
       <c r="D55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C57" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E57">
+        <f>100*AVERAGE(E2:E55)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed 18% of the todo-list
</commit_message>
<xml_diff>
--- a/reviewerTodoList.xlsx
+++ b/reviewerTodoList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukel\Documents\phdThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EDD100-4A19-4255-A022-A185EF36C4FA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D99197-5546-4AB0-8AAF-CBA9505D72EF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6792" xr2:uid="{D14D4B82-700B-4764-8F82-CFD1564063A2}"/>
   </bookViews>
@@ -269,17 +269,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -287,26 +277,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -642,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784CD99F-F0D7-4557-AEAE-23B01A0F6CDF}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -688,7 +658,7 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2">
-        <f>IF(D2,1,0)</f>
+        <f t="shared" ref="F2:F33" si="0">IF(D2,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -708,13 +678,13 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3">
-        <f>IF(D3,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
-        <f t="shared" ref="A4:A55" si="0">A3+1</f>
+        <f t="shared" ref="A4:A55" si="1">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4">
@@ -728,13 +698,13 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4">
-        <f>IF(D4,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B5">
@@ -748,13 +718,13 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5">
-        <f>IF(D5,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B6">
@@ -768,13 +738,13 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6">
-        <f>IF(D6,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B7">
@@ -788,13 +758,13 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7">
-        <f>IF(D7,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B8">
@@ -804,17 +774,17 @@
         <v>9</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8">
-        <f>IF(D8,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B9">
@@ -828,13 +798,13 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9">
-        <f>IF(D9,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B10">
@@ -844,17 +814,17 @@
         <v>11</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10">
-        <f>IF(D10,1,0)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B11">
@@ -868,13 +838,13 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11">
-        <f>IF(D11,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B12">
@@ -888,13 +858,13 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12">
-        <f>IF(D12,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B13">
@@ -908,13 +878,13 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13">
-        <f>IF(D13,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B14">
@@ -928,13 +898,13 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14">
-        <f>IF(D14,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B15">
@@ -948,13 +918,13 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15">
-        <f>IF(D15,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B16">
@@ -968,13 +938,13 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16">
-        <f>IF(D16,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B17">
@@ -988,13 +958,13 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17">
-        <f>IF(D17,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B18">
@@ -1008,13 +978,13 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18">
-        <f>IF(D18,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B19">
@@ -1028,13 +998,13 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19">
-        <f>IF(D19,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B20">
@@ -1048,13 +1018,13 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20">
-        <f>IF(D20,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B21">
@@ -1068,13 +1038,13 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21">
-        <f>IF(D21,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B22">
@@ -1088,13 +1058,13 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22">
-        <f>IF(D22,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B23">
@@ -1108,13 +1078,13 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23">
-        <f>IF(D23,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B24">
@@ -1128,13 +1098,13 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24">
-        <f>IF(D24,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B25">
@@ -1148,13 +1118,13 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25">
-        <f>IF(D25,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B26">
@@ -1168,13 +1138,13 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26">
-        <f>IF(D26,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B27">
@@ -1188,13 +1158,13 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27">
-        <f>IF(D27,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B28">
@@ -1208,13 +1178,13 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28">
-        <f>IF(D28,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B29">
@@ -1228,13 +1198,13 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29">
-        <f>IF(D29,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B30">
@@ -1248,13 +1218,13 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30">
-        <f>IF(D30,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B31">
@@ -1268,13 +1238,13 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31">
-        <f>IF(D31,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B32">
@@ -1288,13 +1258,13 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32">
-        <f>IF(D32,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B33">
@@ -1310,13 +1280,13 @@
         <v>63</v>
       </c>
       <c r="F33">
-        <f>IF(D33,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B34">
@@ -1330,13 +1300,13 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34">
-        <f>IF(D34,1,0)</f>
+        <f t="shared" ref="F34:F55" si="2">IF(D34,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B35">
@@ -1350,13 +1320,13 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35">
-        <f>IF(D35,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B36">
@@ -1370,13 +1340,13 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36">
-        <f>IF(D36,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B37">
@@ -1390,13 +1360,13 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37">
-        <f>IF(D37,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B38">
@@ -1410,13 +1380,13 @@
       </c>
       <c r="E38" s="1"/>
       <c r="F38">
-        <f>IF(D38,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B39">
@@ -1430,13 +1400,13 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39">
-        <f>IF(D39,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B40">
@@ -1450,13 +1420,13 @@
       </c>
       <c r="E40" s="1"/>
       <c r="F40">
-        <f>IF(D40,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B41">
@@ -1470,13 +1440,13 @@
       </c>
       <c r="E41" s="1"/>
       <c r="F41">
-        <f>IF(D41,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B42">
@@ -1490,13 +1460,13 @@
       </c>
       <c r="E42" s="1"/>
       <c r="F42">
-        <f>IF(D42,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B43">
@@ -1510,13 +1480,13 @@
       </c>
       <c r="E43" s="1"/>
       <c r="F43">
-        <f>IF(D43,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B44">
@@ -1532,13 +1502,13 @@
         <v>62</v>
       </c>
       <c r="F44">
-        <f>IF(D44,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B45">
@@ -1552,13 +1522,13 @@
       </c>
       <c r="E45" s="1"/>
       <c r="F45">
-        <f>IF(D45,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B46">
@@ -1572,13 +1542,13 @@
       </c>
       <c r="E46" s="1"/>
       <c r="F46">
-        <f>IF(D46,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B47">
@@ -1592,13 +1562,13 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47">
-        <f>IF(D47,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B48">
@@ -1612,13 +1582,13 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48">
-        <f>IF(D48,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B49">
@@ -1632,13 +1602,13 @@
       </c>
       <c r="E49" s="1"/>
       <c r="F49">
-        <f>IF(D49,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B50">
@@ -1654,13 +1624,13 @@
         <v>59</v>
       </c>
       <c r="F50">
-        <f>IF(D50,1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B51">
@@ -1674,13 +1644,13 @@
       </c>
       <c r="E51" s="1"/>
       <c r="F51">
-        <f>IF(D51,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B52">
@@ -1694,13 +1664,13 @@
       </c>
       <c r="E52" s="1"/>
       <c r="F52">
-        <f>IF(D52,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B53">
@@ -1714,13 +1684,13 @@
       </c>
       <c r="E53" s="1"/>
       <c r="F53">
-        <f>IF(D53,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B54" t="s">
@@ -1734,13 +1704,13 @@
       </c>
       <c r="E54" s="1"/>
       <c r="F54">
-        <f>IF(D54,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B55" t="s">
@@ -1754,7 +1724,7 @@
       </c>
       <c r="E55" s="1"/>
       <c r="F55">
-        <f>IF(D55,1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1764,24 +1734,24 @@
       </c>
       <c r="D57">
         <f>F57</f>
-        <v>14.81</v>
+        <v>18.52</v>
       </c>
       <c r="F57">
         <f>ROUND(100*AVERAGE(F2:F55), 2)</f>
-        <v>14.81</v>
+        <v>18.52</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D38">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D55">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
upto 20% of todolist completed
</commit_message>
<xml_diff>
--- a/reviewerTodoList.xlsx
+++ b/reviewerTodoList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukel\Documents\phdThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D99197-5546-4AB0-8AAF-CBA9505D72EF}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70882D6-E3E7-4057-9CAA-EE51E99D79A4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6792" xr2:uid="{D14D4B82-700B-4764-8F82-CFD1564063A2}"/>
   </bookViews>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784CD99F-F0D7-4557-AEAE-23B01A0F6CDF}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -834,12 +834,12 @@
         <v>12</v>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1734,11 +1734,11 @@
       </c>
       <c r="D57">
         <f>F57</f>
-        <v>18.52</v>
+        <v>20.37</v>
       </c>
       <c r="F57">
         <f>ROUND(100*AVERAGE(F2:F55), 2)</f>
-        <v>18.52</v>
+        <v>20.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upto 27% complete of the todo list
</commit_message>
<xml_diff>
--- a/reviewerTodoList.xlsx
+++ b/reviewerTodoList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukel\Documents\phdThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70882D6-E3E7-4057-9CAA-EE51E99D79A4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829B118B-B7C4-4EFE-AD01-41A0A9A40CEC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6792" xr2:uid="{D14D4B82-700B-4764-8F82-CFD1564063A2}"/>
   </bookViews>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784CD99F-F0D7-4557-AEAE-23B01A0F6CDF}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -694,12 +694,12 @@
         <v>5</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -894,12 +894,12 @@
         <v>15</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1174,12 +1174,12 @@
         <v>28</v>
       </c>
       <c r="D28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1538,12 +1538,12 @@
         <v>47</v>
       </c>
       <c r="D46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1734,11 +1734,11 @@
       </c>
       <c r="D57">
         <f>F57</f>
-        <v>20.37</v>
+        <v>27.78</v>
       </c>
       <c r="F57">
         <f>ROUND(100*AVERAGE(F2:F55), 2)</f>
-        <v>20.37</v>
+        <v>27.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upto 40% of todo list
</commit_message>
<xml_diff>
--- a/reviewerTodoList.xlsx
+++ b/reviewerTodoList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukel\Documents\phdThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829B118B-B7C4-4EFE-AD01-41A0A9A40CEC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE3B47D-3F4D-4215-8B9B-2040EEBF9975}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6792" xr2:uid="{D14D4B82-700B-4764-8F82-CFD1564063A2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>It is already public and will always remain so</t>
+  </si>
+  <si>
+    <t>Already was completed</t>
   </si>
 </sst>
 </file>
@@ -612,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784CD99F-F0D7-4557-AEAE-23B01A0F6CDF}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -654,12 +657,12 @@
         <v>3</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2">
         <f t="shared" ref="F2:F33" si="0">IF(D2,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -854,12 +857,12 @@
         <v>13</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -974,12 +977,12 @@
         <v>19</v>
       </c>
       <c r="D18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1234,12 +1237,12 @@
         <v>32</v>
       </c>
       <c r="D31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1396,12 +1399,12 @@
         <v>40</v>
       </c>
       <c r="D39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1416,12 +1419,14 @@
         <v>41</v>
       </c>
       <c r="D40" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="F40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1720,12 +1725,12 @@
         <v>57</v>
       </c>
       <c r="D55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1734,11 +1739,11 @@
       </c>
       <c r="D57">
         <f>F57</f>
-        <v>27.78</v>
+        <v>40.74</v>
       </c>
       <c r="F57">
         <f>ROUND(100*AVERAGE(F2:F55), 2)</f>
-        <v>27.78</v>
+        <v>40.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
up to 62% complete
</commit_message>
<xml_diff>
--- a/reviewerTodoList.xlsx
+++ b/reviewerTodoList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukel\Documents\phdThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE3B47D-3F4D-4215-8B9B-2040EEBF9975}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8090D36D-09B9-4690-A8C1-1F021A0FEA50}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6792" xr2:uid="{D14D4B82-700B-4764-8F82-CFD1564063A2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
   <si>
     <t>ID</t>
   </si>
@@ -225,6 +225,24 @@
   </si>
   <si>
     <t>Already was completed</t>
+  </si>
+  <si>
+    <t>is this neccesary? I cannot remember every search word I used</t>
+  </si>
+  <si>
+    <t>is this required?</t>
+  </si>
+  <si>
+    <t>references include page numbers, is this required?</t>
+  </si>
+  <si>
+    <t>I cannot find any parts where I do this</t>
+  </si>
+  <si>
+    <t>not having yes answers makes the contributions less than they are</t>
+  </si>
+  <si>
+    <t>Yes, but it was meant to point there, but I can understand the confusion</t>
   </si>
 </sst>
 </file>
@@ -615,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784CD99F-F0D7-4557-AEAE-23B01A0F6CDF}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -717,12 +735,14 @@
         <v>6</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -737,12 +757,12 @@
         <v>7</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
@@ -757,12 +777,12 @@
         <v>8</v>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -785,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -797,12 +817,14 @@
         <v>10</v>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -905,7 +927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -917,12 +939,14 @@
         <v>16</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1017,12 +1041,12 @@
         <v>21</v>
       </c>
       <c r="D20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1429,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -1441,15 +1465,17 @@
         <v>42</v>
       </c>
       <c r="D41" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="F41">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -1461,12 +1487,14 @@
         <v>43</v>
       </c>
       <c r="D42" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="F42">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1481,12 +1509,12 @@
         <v>44</v>
       </c>
       <c r="D43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1563,12 +1591,14 @@
         <v>48</v>
       </c>
       <c r="D47" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="F47">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1685,12 +1715,14 @@
         <v>54</v>
       </c>
       <c r="D53" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="F53">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1705,12 +1737,14 @@
         <v>55</v>
       </c>
       <c r="D54" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="F54">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1739,11 +1773,11 @@
       </c>
       <c r="D57">
         <f>F57</f>
-        <v>40.74</v>
+        <v>62.96</v>
       </c>
       <c r="F57">
         <f>ROUND(100*AVERAGE(F2:F55), 2)</f>
-        <v>40.74</v>
+        <v>62.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
90.74% complete making the changes
</commit_message>
<xml_diff>
--- a/reviewerTodoList.xlsx
+++ b/reviewerTodoList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukel\Documents\phdThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634EFCAC-C566-4D04-80CD-989639E886A0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9FD532-653C-46D1-AF71-6CDE14C6B6C9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6792" xr2:uid="{D14D4B82-700B-4764-8F82-CFD1564063A2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -243,6 +243,18 @@
   </si>
   <si>
     <t>Yes, but it was meant to point there, but I can understand the confusion</t>
+  </si>
+  <si>
+    <t>(added into experiments section intro)</t>
+  </si>
+  <si>
+    <t>(explained in the experiments section)</t>
+  </si>
+  <si>
+    <t>It is in the methodology section, also I explained my rationale behind chosing computational complexity over simple O-analysis</t>
+  </si>
+  <si>
+    <t>alread done in the "Performance Comparison" section</t>
   </si>
 </sst>
 </file>
@@ -633,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784CD99F-F0D7-4557-AEAE-23B01A0F6CDF}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -899,12 +911,12 @@
         <v>14</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -961,12 +973,12 @@
         <v>17</v>
       </c>
       <c r="D16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -981,12 +993,12 @@
         <v>18</v>
       </c>
       <c r="D17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1081,12 +1093,14 @@
         <v>23</v>
       </c>
       <c r="D22" t="b">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1101,15 +1115,17 @@
         <v>24</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1121,12 +1137,14 @@
         <v>25</v>
       </c>
       <c r="D24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1141,12 +1159,12 @@
         <v>31</v>
       </c>
       <c r="D25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1161,12 +1179,12 @@
         <v>26</v>
       </c>
       <c r="D26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1181,12 +1199,12 @@
         <v>27</v>
       </c>
       <c r="D27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1221,12 +1239,12 @@
         <v>29</v>
       </c>
       <c r="D29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1241,12 +1259,14 @@
         <v>30</v>
       </c>
       <c r="D30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1281,12 +1301,12 @@
         <v>33</v>
       </c>
       <c r="D32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1383,12 +1403,12 @@
         <v>38</v>
       </c>
       <c r="D37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1773,11 +1793,11 @@
       </c>
       <c r="D57">
         <f>F57</f>
-        <v>66.67</v>
+        <v>90.74</v>
       </c>
       <c r="F57">
         <f>ROUND(100*AVERAGE(F2:F55), 2)</f>
-        <v>66.67</v>
+        <v>90.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished making the changes, needs one more final overview
</commit_message>
<xml_diff>
--- a/reviewerTodoList.xlsx
+++ b/reviewerTodoList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukel\Documents\phdThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F072697-01D8-4964-AD8C-1963294ABD8C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C3A055-E059-4430-93E5-A5EB93B57D49}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6792" xr2:uid="{D14D4B82-700B-4764-8F82-CFD1564063A2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>I have links in the Table of contents now, but too many equations will compound the thesis too much</t>
+  </si>
+  <si>
+    <t>better sign posting added and overviews added for non-technical readers</t>
+  </si>
+  <si>
+    <t>see item 43</t>
   </si>
 </sst>
 </file>
@@ -648,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784CD99F-F0D7-4557-AEAE-23B01A0F6CDF}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1368,12 +1374,12 @@
         <v>36</v>
       </c>
       <c r="D35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1564,7 +1570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -1576,12 +1582,14 @@
         <v>46</v>
       </c>
       <c r="D45" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="F45">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1700,12 +1708,14 @@
         <v>52</v>
       </c>
       <c r="D51" t="b">
-        <v>0</v>
-      </c>
-      <c r="E51" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="F51">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1720,12 +1730,12 @@
         <v>53</v>
       </c>
       <c r="D52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1798,11 +1808,11 @@
       </c>
       <c r="D57">
         <f>F57</f>
-        <v>92.59</v>
+        <v>100</v>
       </c>
       <c r="F57">
         <f>ROUND(100*AVERAGE(F2:F55), 2)</f>
-        <v>92.59</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>